<commit_message>
- Delete scenario for 08 ApachePOI example
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/recources/ApacheExcel3.xlsx
+++ b/src/test/java/ApachePOI/recources/ApacheExcel3.xlsx
@@ -46,34 +46,34 @@
     <t>End</t>
   </si>
   <si>
-    <t>Us Batw 8 47</t>
-  </si>
-  <si>
-    <t>Us Batw 8 48</t>
-  </si>
-  <si>
-    <t>Us Batw 8 49</t>
-  </si>
-  <si>
-    <t>Us Batw 8 50</t>
-  </si>
-  <si>
-    <t>Us Batw 8 51</t>
-  </si>
-  <si>
-    <t>ubw47</t>
-  </si>
-  <si>
-    <t>ubw48</t>
-  </si>
-  <si>
-    <t>ubw49</t>
-  </si>
-  <si>
-    <t>ubw50</t>
-  </si>
-  <si>
-    <t>ubw51</t>
+    <t>Us Batw 8 58</t>
+  </si>
+  <si>
+    <t>Us Batw 8 59</t>
+  </si>
+  <si>
+    <t>Us Batw 8 60</t>
+  </si>
+  <si>
+    <t>Us Batw 8 61</t>
+  </si>
+  <si>
+    <t>Us Batw 8 62</t>
+  </si>
+  <si>
+    <t>ubw58</t>
+  </si>
+  <si>
+    <t>ubw59</t>
+  </si>
+  <si>
+    <t>ubw60</t>
+  </si>
+  <si>
+    <t>ubw61</t>
+  </si>
+  <si>
+    <t>ubw62</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>